<commit_message>
Made slides for presentation
</commit_message>
<xml_diff>
--- a/excel/DnaTest.xlsx
+++ b/excel/DnaTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8145" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -5329,11 +5329,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496802472"/>
-        <c:axId val="496799336"/>
+        <c:axId val="250743880"/>
+        <c:axId val="250741528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496802472"/>
+        <c:axId val="250743880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5423,7 +5423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496799336"/>
+        <c:crossAx val="250741528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -5433,7 +5433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496799336"/>
+        <c:axId val="250741528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="90"/>
@@ -5532,7 +5532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496802472"/>
+        <c:crossAx val="250743880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12360,11 +12360,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="501112448"/>
-        <c:axId val="501112840"/>
+        <c:axId val="503428760"/>
+        <c:axId val="503429544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="501112448"/>
+        <c:axId val="503428760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12463,7 +12463,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501112840"/>
+        <c:crossAx val="503429544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12472,7 +12472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="501112840"/>
+        <c:axId val="503429544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12579,7 +12579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501112448"/>
+        <c:crossAx val="503428760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19410,11 +19410,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="500344864"/>
-        <c:axId val="500347608"/>
+        <c:axId val="502883552"/>
+        <c:axId val="502887472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="500344864"/>
+        <c:axId val="502883552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19513,7 +19513,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500347608"/>
+        <c:crossAx val="502887472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19523,7 +19523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="500347608"/>
+        <c:axId val="502887472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19630,7 +19630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500344864"/>
+        <c:crossAx val="502883552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21704,7 +21704,7 @@
   <dimension ref="A1:M238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22317,7 +22317,7 @@
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B3:L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25886,8 +25886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30705,8 +30705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>